<commit_message>
Few changes to the code to adapt the env
</commit_message>
<xml_diff>
--- a/Experiment Arrangements.xlsx
+++ b/Experiment Arrangements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Ruoyu MT\MasterThesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ruoyu\MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7197AB11-6DF7-4E76-8223-0996007A4FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF783348-7867-4508-B77B-26938C3046C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
   <si>
     <t>Col1</t>
   </si>
@@ -254,13 +254,23 @@
   </si>
   <si>
     <t>17.Mar 18:00</t>
+  </si>
+  <si>
+    <t>Clip</t>
+  </si>
+  <si>
+    <t>S = sad, A = angry, H = happy, E = exciting
+v = video, a = audio, i = image, r = autobiographical-recall</t>
+  </si>
+  <si>
+    <t>12.Jun 17:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,8 +315,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,8 +343,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -517,16 +547,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -563,10 +607,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -844,88 +896,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="22" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="N1" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="12">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
-        <v>1</v>
-      </c>
-      <c r="J2" s="13">
-        <v>2</v>
-      </c>
-      <c r="K2" s="14">
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
+      <c r="J2" s="11">
+        <v>2</v>
+      </c>
+      <c r="K2" s="12">
         <v>3</v>
       </c>
-      <c r="N2" s="7">
-        <v>1</v>
-      </c>
-      <c r="O2" s="8">
-        <v>1</v>
-      </c>
-      <c r="P2" s="9">
+      <c r="N2" s="5">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
+      <c r="P2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -934,13 +995,13 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <v>4</v>
       </c>
       <c r="I3" s="1">
@@ -949,24 +1010,24 @@
       <c r="J3" s="1">
         <v>6</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="14">
         <v>7</v>
       </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2">
+      <c r="N3" s="37">
+        <v>1</v>
+      </c>
+      <c r="O3" s="38">
+        <v>1</v>
+      </c>
+      <c r="P3" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -975,13 +1036,13 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>8</v>
       </c>
       <c r="I4" s="1">
@@ -990,127 +1051,127 @@
       <c r="J4" s="1">
         <v>10</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="14">
         <v>11</v>
       </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>2</v>
-      </c>
-      <c r="P4" s="2">
+      <c r="N4" s="37">
+        <v>1</v>
+      </c>
+      <c r="O4" s="38">
+        <v>2</v>
+      </c>
+      <c r="P4" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="15">
         <v>12</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="16">
         <v>13</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="16">
         <v>14</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="17">
         <v>15</v>
       </c>
-      <c r="N5" s="3">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>2</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="N5" s="37">
+        <v>1</v>
+      </c>
+      <c r="O5" s="38">
+        <v>2</v>
+      </c>
+      <c r="P5" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="16"/>
-      <c r="G6" s="17"/>
+      <c r="E6" s="14"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="16"/>
-      <c r="N6" s="3">
-        <v>2</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="2">
+      <c r="K6" s="14"/>
+      <c r="N6" s="37">
+        <v>2</v>
+      </c>
+      <c r="O6" s="38">
+        <v>1</v>
+      </c>
+      <c r="P6" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="23">
-        <v>0</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="21">
+        <v>0</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0</v>
-      </c>
-      <c r="I7" s="13">
-        <v>1</v>
-      </c>
-      <c r="J7" s="13">
-        <v>2</v>
-      </c>
-      <c r="K7" s="14">
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2</v>
+      </c>
+      <c r="K7" s="12">
         <v>3</v>
       </c>
-      <c r="N7" s="3">
-        <v>2</v>
-      </c>
-      <c r="O7" s="1">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
+      <c r="N7" s="37">
+        <v>2</v>
+      </c>
+      <c r="O7" s="38">
+        <v>1</v>
+      </c>
+      <c r="P7" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="23">
-        <v>1</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1119,13 +1180,13 @@
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="23">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
+      <c r="G8" s="21">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
         <v>4</v>
       </c>
       <c r="I8" s="1">
@@ -1134,24 +1195,24 @@
       <c r="J8" s="1">
         <v>6</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="14">
         <v>7</v>
       </c>
-      <c r="N8" s="3">
-        <v>2</v>
-      </c>
-      <c r="O8" s="1">
-        <v>2</v>
-      </c>
-      <c r="P8" s="2">
+      <c r="N8" s="37">
+        <v>2</v>
+      </c>
+      <c r="O8" s="38">
+        <v>2</v>
+      </c>
+      <c r="P8" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="23">
-        <v>2</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="21">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1160,13 +1221,13 @@
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="23">
-        <v>2</v>
-      </c>
-      <c r="H9" s="15">
+      <c r="G9" s="21">
+        <v>2</v>
+      </c>
+      <c r="H9" s="13">
         <v>8</v>
       </c>
       <c r="I9" s="1">
@@ -1175,24 +1236,24 @@
       <c r="J9" s="1">
         <v>10</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="14">
         <v>11</v>
       </c>
-      <c r="N9" s="4">
-        <v>2</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2</v>
-      </c>
-      <c r="P9" s="6">
+      <c r="N9" s="2">
+        <v>2</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2</v>
+      </c>
+      <c r="P9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="23">
+      <c r="A10" s="21">
         <v>3</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1201,13 +1262,13 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="21">
         <v>3</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="13">
         <v>12</v>
       </c>
       <c r="I10" s="1">
@@ -1216,15 +1277,15 @@
       <c r="J10" s="1">
         <v>14</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="23">
+      <c r="A11" s="21">
         <v>4</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1233,13 +1294,13 @@
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="21">
         <v>4</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <f>H2</f>
         <v>0</v>
       </c>
@@ -1251,16 +1312,16 @@
         <f>H4</f>
         <v>8</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="14">
         <f>H5</f>
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="23">
+      <c r="A12" s="21">
         <v>5</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1269,13 +1330,13 @@
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="21">
         <v>5</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="13">
         <v>1</v>
       </c>
       <c r="I12" s="1">
@@ -1284,15 +1345,15 @@
       <c r="J12" s="1">
         <v>9</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="14">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="23">
+      <c r="A13" s="21">
         <v>6</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1301,13 +1362,13 @@
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="21">
         <v>6</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="13">
         <v>2</v>
       </c>
       <c r="I13" s="1">
@@ -1316,15 +1377,15 @@
       <c r="J13" s="1">
         <v>10</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="14">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="23">
+      <c r="A14" s="21">
         <v>7</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1333,13 +1394,13 @@
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="21">
         <v>7</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="13">
         <v>3</v>
       </c>
       <c r="I14" s="1">
@@ -1348,15 +1409,15 @@
       <c r="J14" s="1">
         <v>11</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="14">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="23">
+      <c r="A15" s="21">
         <v>8</v>
       </c>
-      <c r="B15" s="15" t="str">
+      <c r="B15" s="13" t="str">
         <f>E2</f>
         <v>Er</v>
       </c>
@@ -1368,14 +1429,14 @@
         <f>C2</f>
         <v>Aa</v>
       </c>
-      <c r="E15" s="16" t="str">
+      <c r="E15" s="14" t="str">
         <f>B2</f>
         <v>Sv</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="21">
         <v>8</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="13">
         <f>K2</f>
         <v>3</v>
       </c>
@@ -1387,16 +1448,16 @@
         <f>I2</f>
         <v>1</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="14">
         <f>H2</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="23">
+      <c r="A16" s="21">
         <v>9</v>
       </c>
-      <c r="B16" s="15" t="str">
+      <c r="B16" s="13" t="str">
         <f t="shared" ref="B16:B18" si="0">E3</f>
         <v>Si</v>
       </c>
@@ -1408,14 +1469,14 @@
         <f t="shared" ref="D16:D18" si="2">C3</f>
         <v>Hv</v>
       </c>
-      <c r="E16" s="16" t="str">
+      <c r="E16" s="14" t="str">
         <f t="shared" ref="E16:E18" si="3">B3</f>
         <v>Ar</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="21">
         <v>9</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="13">
         <f t="shared" ref="H16:H18" si="4">K3</f>
         <v>7</v>
       </c>
@@ -1427,16 +1488,16 @@
         <f t="shared" ref="J16:J18" si="6">I3</f>
         <v>5</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="14">
         <f t="shared" ref="K16:K18" si="7">H3</f>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="23">
+    <row r="17" spans="1:17">
+      <c r="A17" s="21">
         <v>10</v>
       </c>
-      <c r="B17" s="15" t="str">
+      <c r="B17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Av</v>
       </c>
@@ -1448,14 +1509,14 @@
         <f t="shared" si="2"/>
         <v>Ei</v>
       </c>
-      <c r="E17" s="16" t="str">
+      <c r="E17" s="14" t="str">
         <f t="shared" si="3"/>
         <v>Ha</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="21">
         <v>10</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="13">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
@@ -1467,16 +1528,21 @@
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="14">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="23">
+      <c r="O17" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="21">
         <v>11</v>
       </c>
-      <c r="B18" s="15" t="str">
+      <c r="B18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Ha</v>
       </c>
@@ -1488,14 +1554,14 @@
         <f t="shared" si="2"/>
         <v>Sr</v>
       </c>
-      <c r="E18" s="16" t="str">
+      <c r="E18" s="14" t="str">
         <f t="shared" si="3"/>
         <v>Ei</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="21">
         <v>11</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="13">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
@@ -1507,16 +1573,19 @@
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="14">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="23">
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="21">
         <v>12</v>
       </c>
-      <c r="B19" s="15" t="str">
+      <c r="B19" s="13" t="str">
         <f>E11</f>
         <v>Ei</v>
       </c>
@@ -1528,14 +1597,14 @@
         <f>C11</f>
         <v>Ar</v>
       </c>
-      <c r="E19" s="16" t="str">
+      <c r="E19" s="14" t="str">
         <f>B11</f>
         <v>Sv</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="21">
         <v>12</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="13">
         <f>K11</f>
         <v>12</v>
       </c>
@@ -1547,16 +1616,19 @@
         <f>I11</f>
         <v>4</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="14">
         <f>H11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="23">
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="21">
         <v>13</v>
       </c>
-      <c r="B20" s="15" t="str">
+      <c r="B20" s="13" t="str">
         <f t="shared" ref="B20:B22" si="8">E12</f>
         <v>Sr</v>
       </c>
@@ -1568,14 +1640,14 @@
         <f t="shared" ref="D20:D22" si="10">C12</f>
         <v>Hv</v>
       </c>
-      <c r="E20" s="16" t="str">
+      <c r="E20" s="14" t="str">
         <f t="shared" ref="E20:E22" si="11">B12</f>
         <v>Aa</v>
       </c>
-      <c r="G20" s="23">
+      <c r="G20" s="21">
         <v>13</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="13">
         <f t="shared" ref="H20:H22" si="12">K12</f>
         <v>13</v>
       </c>
@@ -1587,16 +1659,19 @@
         <f t="shared" ref="J20:J22" si="14">I12</f>
         <v>5</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="14">
         <f t="shared" ref="K20:K22" si="15">H12</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="23">
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="21">
         <v>14</v>
       </c>
-      <c r="B21" s="15" t="str">
+      <c r="B21" s="13" t="str">
         <f t="shared" si="8"/>
         <v>Av</v>
       </c>
@@ -1608,14 +1683,14 @@
         <f t="shared" si="10"/>
         <v>Ea</v>
       </c>
-      <c r="E21" s="16" t="str">
+      <c r="E21" s="14" t="str">
         <f t="shared" si="11"/>
         <v>Hi</v>
       </c>
-      <c r="G21" s="23">
+      <c r="G21" s="21">
         <v>14</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="13">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
@@ -1627,52 +1702,58 @@
         <f t="shared" si="14"/>
         <v>6</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="14">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="24">
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="22">
         <v>15</v>
       </c>
-      <c r="B22" s="17" t="str">
+      <c r="B22" s="15" t="str">
         <f t="shared" si="8"/>
         <v>Ha</v>
       </c>
-      <c r="C22" s="18" t="str">
+      <c r="C22" s="16" t="str">
         <f t="shared" si="9"/>
         <v>Av</v>
       </c>
-      <c r="D22" s="18" t="str">
+      <c r="D22" s="16" t="str">
         <f t="shared" si="10"/>
         <v>Si</v>
       </c>
-      <c r="E22" s="19" t="str">
+      <c r="E22" s="17" t="str">
         <f t="shared" si="11"/>
         <v>Er</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="22">
         <v>15</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="15">
         <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="16">
         <f t="shared" si="13"/>
         <v>11</v>
       </c>
-      <c r="J22" s="18">
+      <c r="J22" s="16">
         <f t="shared" si="14"/>
         <v>7</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="17">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O17:Q21"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1684,8 +1765,8 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1694,156 +1775,156 @@
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="25"/>
+    <col min="5" max="5" width="9.140625" style="23"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="26" customFormat="1">
-      <c r="A2" s="26">
-        <v>1</v>
-      </c>
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:10" s="24" customFormat="1">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="26">
-        <v>1</v>
-      </c>
-      <c r="E2" s="33">
-        <v>0</v>
-      </c>
-      <c r="F2" s="26">
-        <v>1</v>
-      </c>
-      <c r="G2" s="26">
-        <v>1</v>
-      </c>
-      <c r="H2" s="26">
-        <v>1</v>
-      </c>
-      <c r="I2" s="26" t="s">
+      <c r="D2" s="24">
+        <v>1</v>
+      </c>
+      <c r="E2" s="31">
+        <v>0</v>
+      </c>
+      <c r="F2" s="24">
+        <v>1</v>
+      </c>
+      <c r="G2" s="24">
+        <v>1</v>
+      </c>
+      <c r="H2" s="24">
+        <v>1</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="28" customFormat="1">
-      <c r="A3" s="28">
-        <v>1</v>
-      </c>
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="1:10" s="26" customFormat="1">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="28">
-        <v>0</v>
-      </c>
-      <c r="E3" s="34">
-        <v>0</v>
-      </c>
-      <c r="F3" s="28">
-        <v>2</v>
-      </c>
-      <c r="G3" s="28">
-        <v>2</v>
-      </c>
-      <c r="H3" s="28">
-        <v>2</v>
-      </c>
-      <c r="I3" s="28" t="s">
+      <c r="D3" s="26">
+        <v>0</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0</v>
+      </c>
+      <c r="F3" s="26">
+        <v>2</v>
+      </c>
+      <c r="G3" s="26">
+        <v>2</v>
+      </c>
+      <c r="H3" s="26">
+        <v>2</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="26" customFormat="1">
-      <c r="A4" s="26">
-        <v>2</v>
-      </c>
-      <c r="B4" s="26" t="s">
+    <row r="4" spans="1:10" s="24" customFormat="1">
+      <c r="A4" s="24">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="26">
-        <v>1</v>
-      </c>
-      <c r="E4" s="33">
-        <v>1</v>
-      </c>
-      <c r="F4" s="26">
-        <v>1</v>
-      </c>
-      <c r="G4" s="26">
-        <v>1</v>
-      </c>
-      <c r="H4" s="26">
-        <v>1</v>
-      </c>
-      <c r="I4" s="26" t="s">
+      <c r="D4" s="24">
+        <v>1</v>
+      </c>
+      <c r="E4" s="31">
+        <v>1</v>
+      </c>
+      <c r="F4" s="24">
+        <v>1</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1</v>
+      </c>
+      <c r="H4" s="24">
+        <v>1</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="28" customFormat="1">
-      <c r="A5" s="28">
-        <v>2</v>
-      </c>
-      <c r="B5" s="28" t="s">
+    <row r="5" spans="1:10" s="26" customFormat="1">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="28">
-        <v>0</v>
-      </c>
-      <c r="E5" s="34">
-        <v>1</v>
-      </c>
-      <c r="F5" s="28">
-        <v>2</v>
-      </c>
-      <c r="G5" s="28">
-        <v>2</v>
-      </c>
-      <c r="H5" s="28">
-        <v>2</v>
-      </c>
-      <c r="I5" s="28" t="s">
+      <c r="D5" s="26">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>2</v>
+      </c>
+      <c r="G5" s="26">
+        <v>2</v>
+      </c>
+      <c r="H5" s="26">
+        <v>2</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1854,7 +1935,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>2</v>
       </c>
       <c r="F6">
@@ -1874,7 +1955,7 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>2</v>
       </c>
       <c r="F7">
@@ -1887,380 +1968,380 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="30" customFormat="1">
-      <c r="A8" s="30">
+    <row r="8" spans="1:10" s="28" customFormat="1">
+      <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="30">
-        <v>1</v>
-      </c>
-      <c r="E8" s="35">
+      <c r="D8" s="28">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33">
         <v>3</v>
       </c>
-      <c r="F8" s="30">
-        <v>1</v>
-      </c>
-      <c r="G8" s="30">
-        <v>1</v>
-      </c>
-      <c r="H8" s="30">
-        <v>1</v>
-      </c>
-      <c r="I8" s="30" t="s">
+      <c r="F8" s="28">
+        <v>1</v>
+      </c>
+      <c r="G8" s="28">
+        <v>1</v>
+      </c>
+      <c r="H8" s="28">
+        <v>1</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="26" customFormat="1">
-      <c r="A9" s="26">
+    <row r="9" spans="1:10" s="24" customFormat="1">
+      <c r="A9" s="24">
         <v>4</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="26">
-        <v>0</v>
-      </c>
-      <c r="E9" s="26">
+      <c r="D9" s="24">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24">
         <v>3</v>
       </c>
-      <c r="F9" s="26">
-        <v>2</v>
-      </c>
-      <c r="G9" s="26">
-        <v>2</v>
-      </c>
-      <c r="H9" s="26">
-        <v>2</v>
-      </c>
-      <c r="I9" s="26" t="s">
+      <c r="F9" s="24">
+        <v>2</v>
+      </c>
+      <c r="G9" s="24">
+        <v>2</v>
+      </c>
+      <c r="H9" s="24">
+        <v>2</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="26" customFormat="1">
-      <c r="A10" s="26">
+    <row r="10" spans="1:10" s="24" customFormat="1">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="26">
-        <v>1</v>
-      </c>
-      <c r="E10" s="33">
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
+      <c r="E10" s="31">
         <v>4</v>
       </c>
-      <c r="F10" s="26">
-        <v>1</v>
-      </c>
-      <c r="G10" s="26">
-        <v>1</v>
-      </c>
-      <c r="H10" s="26">
-        <v>1</v>
-      </c>
-      <c r="I10" s="26" t="s">
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24">
+        <v>1</v>
+      </c>
+      <c r="I10" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="30" customFormat="1">
-      <c r="A11" s="30">
+    <row r="11" spans="1:10" s="28" customFormat="1">
+      <c r="A11" s="28">
         <v>5</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="30">
-        <v>0</v>
-      </c>
-      <c r="E11" s="35">
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
         <v>4</v>
       </c>
-      <c r="F11" s="30">
-        <v>2</v>
-      </c>
-      <c r="G11" s="30">
-        <v>2</v>
-      </c>
-      <c r="H11" s="30">
-        <v>2</v>
-      </c>
-      <c r="I11" s="30" t="s">
+      <c r="F11" s="28">
+        <v>2</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2</v>
+      </c>
+      <c r="H11" s="28">
+        <v>2</v>
+      </c>
+      <c r="I11" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="26" customFormat="1">
-      <c r="A12" s="26">
+    <row r="12" spans="1:10" s="24" customFormat="1">
+      <c r="A12" s="24">
         <v>6</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="26">
-        <v>1</v>
-      </c>
-      <c r="E12" s="33">
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="31">
         <v>5</v>
       </c>
-      <c r="F12" s="26">
-        <v>1</v>
-      </c>
-      <c r="G12" s="26">
-        <v>1</v>
-      </c>
-      <c r="H12" s="26">
-        <v>1</v>
-      </c>
-      <c r="I12" s="26" t="s">
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="24">
+        <v>1</v>
+      </c>
+      <c r="H12" s="24">
+        <v>1</v>
+      </c>
+      <c r="I12" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="30" customFormat="1">
-      <c r="A13" s="30">
+    <row r="13" spans="1:10" s="28" customFormat="1">
+      <c r="A13" s="28">
         <v>6</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="30">
-        <v>0</v>
-      </c>
-      <c r="E13" s="35">
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
         <v>5</v>
       </c>
-      <c r="F13" s="30">
-        <v>2</v>
-      </c>
-      <c r="G13" s="30">
-        <v>2</v>
-      </c>
-      <c r="H13" s="30">
-        <v>2</v>
-      </c>
-      <c r="I13" s="30" t="s">
+      <c r="F13" s="28">
+        <v>2</v>
+      </c>
+      <c r="G13" s="28">
+        <v>2</v>
+      </c>
+      <c r="H13" s="28">
+        <v>2</v>
+      </c>
+      <c r="I13" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="28" customFormat="1">
-      <c r="A14" s="28">
+    <row r="14" spans="1:10" s="26" customFormat="1">
+      <c r="A14" s="26">
         <v>7</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="28">
-        <v>1</v>
-      </c>
-      <c r="E14" s="34">
+      <c r="D14" s="26">
+        <v>1</v>
+      </c>
+      <c r="E14" s="32">
         <v>6</v>
       </c>
-      <c r="F14" s="28">
-        <v>1</v>
-      </c>
-      <c r="G14" s="28">
-        <v>1</v>
-      </c>
-      <c r="H14" s="28">
-        <v>1</v>
-      </c>
-      <c r="I14" s="28" t="s">
+      <c r="F14" s="26">
+        <v>1</v>
+      </c>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1</v>
+      </c>
+      <c r="I14" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="30" customFormat="1">
-      <c r="A15" s="30">
+    <row r="15" spans="1:10" s="28" customFormat="1">
+      <c r="A15" s="28">
         <v>7</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="30">
-        <v>0</v>
-      </c>
-      <c r="E15" s="35">
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="33">
         <v>6</v>
       </c>
-      <c r="F15" s="30">
-        <v>2</v>
-      </c>
-      <c r="G15" s="30">
-        <v>2</v>
-      </c>
-      <c r="H15" s="30">
-        <v>2</v>
-      </c>
-      <c r="I15" s="30" t="s">
+      <c r="F15" s="28">
+        <v>2</v>
+      </c>
+      <c r="G15" s="28">
+        <v>2</v>
+      </c>
+      <c r="H15" s="28">
+        <v>2</v>
+      </c>
+      <c r="I15" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="30" customFormat="1">
-      <c r="A16" s="30">
+    <row r="16" spans="1:10" s="28" customFormat="1">
+      <c r="A16" s="28">
         <v>8</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="30">
-        <v>1</v>
-      </c>
-      <c r="E16" s="35">
+      <c r="D16" s="28">
+        <v>1</v>
+      </c>
+      <c r="E16" s="33">
         <v>7</v>
       </c>
-      <c r="F16" s="30">
-        <v>1</v>
-      </c>
-      <c r="G16" s="30">
-        <v>1</v>
-      </c>
-      <c r="H16" s="30">
-        <v>1</v>
-      </c>
-      <c r="I16" s="30" t="s">
+      <c r="F16" s="28">
+        <v>1</v>
+      </c>
+      <c r="G16" s="28">
+        <v>1</v>
+      </c>
+      <c r="H16" s="28">
+        <v>1</v>
+      </c>
+      <c r="I16" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="30" customFormat="1">
-      <c r="A17" s="30">
+    <row r="17" spans="1:10" s="28" customFormat="1">
+      <c r="A17" s="28">
         <v>8</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="30">
-        <v>0</v>
-      </c>
-      <c r="E17" s="35">
+      <c r="D17" s="28">
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
         <v>7</v>
       </c>
-      <c r="F17" s="30">
-        <v>2</v>
-      </c>
-      <c r="G17" s="30">
-        <v>2</v>
-      </c>
-      <c r="H17" s="30">
-        <v>2</v>
-      </c>
-      <c r="I17" s="30" t="s">
+      <c r="F17" s="28">
+        <v>2</v>
+      </c>
+      <c r="G17" s="28">
+        <v>2</v>
+      </c>
+      <c r="H17" s="28">
+        <v>2</v>
+      </c>
+      <c r="I17" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="28" customFormat="1">
-      <c r="A18" s="28">
+    <row r="18" spans="1:10" s="26" customFormat="1">
+      <c r="A18" s="26">
         <v>9</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="28">
-        <v>1</v>
-      </c>
-      <c r="E18" s="34">
+      <c r="D18" s="26">
+        <v>1</v>
+      </c>
+      <c r="E18" s="32">
         <v>8</v>
       </c>
-      <c r="F18" s="28">
-        <v>1</v>
-      </c>
-      <c r="G18" s="28">
-        <v>1</v>
-      </c>
-      <c r="H18" s="28">
-        <v>1</v>
-      </c>
-      <c r="I18" s="28" t="s">
+      <c r="F18" s="26">
+        <v>1</v>
+      </c>
+      <c r="G18" s="26">
+        <v>1</v>
+      </c>
+      <c r="H18" s="26">
+        <v>1</v>
+      </c>
+      <c r="I18" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="30" customFormat="1">
-      <c r="A19" s="30">
+    <row r="19" spans="1:10" s="28" customFormat="1">
+      <c r="A19" s="28">
         <v>9</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="30">
-        <v>0</v>
-      </c>
-      <c r="E19" s="35">
+      <c r="D19" s="28">
+        <v>0</v>
+      </c>
+      <c r="E19" s="33">
         <v>8</v>
       </c>
-      <c r="F19" s="30">
-        <v>2</v>
-      </c>
-      <c r="G19" s="30">
-        <v>2</v>
-      </c>
-      <c r="H19" s="30">
-        <v>2</v>
-      </c>
-      <c r="I19" s="30" t="s">
+      <c r="F19" s="28">
+        <v>2</v>
+      </c>
+      <c r="G19" s="28">
+        <v>2</v>
+      </c>
+      <c r="H19" s="28">
+        <v>2</v>
+      </c>
+      <c r="I19" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="26" customFormat="1">
-      <c r="A20" s="26">
+    <row r="20" spans="1:10" s="24" customFormat="1">
+      <c r="A20" s="24">
         <v>10</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="26">
-        <v>1</v>
-      </c>
-      <c r="E20" s="33">
+      <c r="D20" s="24">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31">
         <v>9</v>
       </c>
-      <c r="F20" s="26">
-        <v>1</v>
-      </c>
-      <c r="G20" s="26">
-        <v>1</v>
-      </c>
-      <c r="H20" s="26">
-        <v>1</v>
-      </c>
-      <c r="I20" s="26" t="s">
+      <c r="F20" s="24">
+        <v>1</v>
+      </c>
+      <c r="G20" s="24">
+        <v>1</v>
+      </c>
+      <c r="H20" s="24">
+        <v>1</v>
+      </c>
+      <c r="I20" s="24" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2274,7 +2355,7 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="23">
         <v>9</v>
       </c>
       <c r="F21">
@@ -2286,34 +2367,34 @@
       <c r="H21">
         <v>2</v>
       </c>
-      <c r="J21" s="25"/>
-    </row>
-    <row r="22" spans="1:10" s="30" customFormat="1">
-      <c r="A22" s="30">
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="1:10" s="28" customFormat="1">
+      <c r="A22" s="28">
         <v>11</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="30">
-        <v>1</v>
-      </c>
-      <c r="E22" s="35">
+      <c r="D22" s="28">
+        <v>1</v>
+      </c>
+      <c r="E22" s="33">
         <v>10</v>
       </c>
-      <c r="F22" s="30">
-        <v>1</v>
-      </c>
-      <c r="G22" s="30">
-        <v>1</v>
-      </c>
-      <c r="H22" s="30">
-        <v>1</v>
-      </c>
-      <c r="I22" s="30" t="s">
+      <c r="F22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="28">
+        <v>1</v>
+      </c>
+      <c r="H22" s="28">
+        <v>1</v>
+      </c>
+      <c r="I22" s="28" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2321,13 +2402,13 @@
       <c r="A23">
         <v>11</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="25" t="s">
         <v>65</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="23">
         <v>10</v>
       </c>
       <c r="F23">
@@ -2340,32 +2421,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="30" customFormat="1">
-      <c r="A24" s="30">
+    <row r="24" spans="1:10" s="28" customFormat="1">
+      <c r="A24" s="28">
         <v>12</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="30">
-        <v>1</v>
-      </c>
-      <c r="E24" s="35">
+      <c r="D24" s="28">
+        <v>1</v>
+      </c>
+      <c r="E24" s="33">
         <v>11</v>
       </c>
-      <c r="F24" s="30">
-        <v>1</v>
-      </c>
-      <c r="G24" s="30">
-        <v>1</v>
-      </c>
-      <c r="H24" s="30">
-        <v>1</v>
-      </c>
-      <c r="I24" s="30" t="s">
+      <c r="F24" s="28">
+        <v>1</v>
+      </c>
+      <c r="G24" s="28">
+        <v>1</v>
+      </c>
+      <c r="H24" s="28">
+        <v>1</v>
+      </c>
+      <c r="I24" s="28" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2373,13 +2454,13 @@
       <c r="A25">
         <v>12</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="25" t="s">
         <v>67</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="23">
         <v>11</v>
       </c>
       <c r="F25">
@@ -2392,61 +2473,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="28" customFormat="1">
-      <c r="A26" s="28">
+    <row r="26" spans="1:10" s="26" customFormat="1">
+      <c r="A26" s="26">
         <v>13</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="28">
-        <v>1</v>
-      </c>
-      <c r="E26" s="34">
+      <c r="D26" s="26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="32">
         <v>12</v>
       </c>
-      <c r="F26" s="28">
-        <v>1</v>
-      </c>
-      <c r="G26" s="28">
-        <v>1</v>
-      </c>
-      <c r="H26" s="28">
-        <v>1</v>
-      </c>
-      <c r="I26" s="28" t="s">
+      <c r="F26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <v>1</v>
+      </c>
+      <c r="H26" s="26">
+        <v>1</v>
+      </c>
+      <c r="I26" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="26" customFormat="1">
-      <c r="A27" s="26">
+    <row r="27" spans="1:10" s="24" customFormat="1">
+      <c r="A27" s="24">
         <v>13</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="26">
-        <v>0</v>
-      </c>
-      <c r="E27" s="26">
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="24">
         <v>12</v>
       </c>
-      <c r="F27" s="26">
-        <v>2</v>
-      </c>
-      <c r="G27" s="26">
-        <v>2</v>
-      </c>
-      <c r="H27" s="26">
-        <v>2</v>
-      </c>
-      <c r="I27" s="26" t="s">
+      <c r="F27" s="24">
+        <v>2</v>
+      </c>
+      <c r="G27" s="24">
+        <v>2</v>
+      </c>
+      <c r="H27" s="24">
+        <v>2</v>
+      </c>
+      <c r="I27" s="24" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2457,7 +2538,7 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="23">
         <v>13</v>
       </c>
       <c r="F28">
@@ -2477,7 +2558,7 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="23">
         <v>13</v>
       </c>
       <c r="F29">
@@ -2490,32 +2571,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="26" customFormat="1">
-      <c r="A30" s="26">
+    <row r="30" spans="1:10" s="24" customFormat="1">
+      <c r="A30" s="24">
         <v>15</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="26">
-        <v>1</v>
-      </c>
-      <c r="E30" s="33">
+      <c r="D30" s="24">
+        <v>1</v>
+      </c>
+      <c r="E30" s="31">
         <v>14</v>
       </c>
-      <c r="F30" s="26">
-        <v>1</v>
-      </c>
-      <c r="G30" s="26">
-        <v>1</v>
-      </c>
-      <c r="H30" s="26">
-        <v>1</v>
-      </c>
-      <c r="I30" s="26" t="s">
+      <c r="F30" s="24">
+        <v>1</v>
+      </c>
+      <c r="G30" s="24">
+        <v>1</v>
+      </c>
+      <c r="H30" s="24">
+        <v>1</v>
+      </c>
+      <c r="I30" s="24" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2532,7 +2613,7 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="23">
         <v>14</v>
       </c>
       <c r="F31">
@@ -2545,104 +2626,107 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="30" customFormat="1">
-      <c r="A32" s="30">
+    <row r="32" spans="1:10" s="28" customFormat="1">
+      <c r="A32" s="28">
         <v>16</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="30">
-        <v>1</v>
-      </c>
-      <c r="E32" s="30">
+      <c r="D32" s="28">
+        <v>1</v>
+      </c>
+      <c r="E32" s="28">
         <v>15</v>
       </c>
-      <c r="F32" s="30">
-        <v>1</v>
-      </c>
-      <c r="G32" s="30">
-        <v>1</v>
-      </c>
-      <c r="H32" s="30">
-        <v>1</v>
-      </c>
-      <c r="I32" s="30" t="s">
+      <c r="F32" s="28">
+        <v>1</v>
+      </c>
+      <c r="G32" s="28">
+        <v>1</v>
+      </c>
+      <c r="H32" s="28">
+        <v>1</v>
+      </c>
+      <c r="I32" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="26" customFormat="1">
-      <c r="A33" s="26">
+    <row r="33" spans="1:9" s="24" customFormat="1">
+      <c r="A33" s="24">
         <v>16</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="26">
-        <v>0</v>
-      </c>
-      <c r="E33" s="26">
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="24">
         <v>15</v>
       </c>
-      <c r="F33" s="26">
-        <v>2</v>
-      </c>
-      <c r="G33" s="26">
-        <v>2</v>
-      </c>
-      <c r="H33" s="26">
-        <v>2</v>
-      </c>
-      <c r="I33" s="26" t="s">
+      <c r="F33" s="24">
+        <v>2</v>
+      </c>
+      <c r="G33" s="24">
+        <v>2</v>
+      </c>
+      <c r="H33" s="24">
+        <v>2</v>
+      </c>
+      <c r="I33" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="31" customFormat="1">
-      <c r="A34" s="31">
+    <row r="34" spans="1:9" s="29" customFormat="1">
+      <c r="A34" s="29">
         <v>17</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="31">
-        <v>0</v>
-      </c>
-      <c r="E34" s="36">
-        <v>0</v>
-      </c>
-      <c r="F34" s="31">
-        <v>2</v>
-      </c>
-      <c r="G34" s="31">
-        <v>2</v>
-      </c>
-      <c r="H34" s="31">
-        <v>2</v>
-      </c>
-      <c r="I34" s="31" t="s">
+      <c r="D34" s="29">
+        <v>0</v>
+      </c>
+      <c r="E34" s="34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="29">
+        <v>2</v>
+      </c>
+      <c r="G34" s="29">
+        <v>2</v>
+      </c>
+      <c r="H34" s="29">
+        <v>2</v>
+      </c>
+      <c r="I34" s="29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35">
+    <row r="35" spans="1:9" s="24" customFormat="1">
+      <c r="A35" s="24">
         <v>17</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="25">
+      <c r="C35" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="24">
+        <v>1</v>
+      </c>
+      <c r="E35" s="24">
         <v>0</v>
       </c>
       <c r="F35" s="27">
@@ -2653,6 +2737,9 @@
       </c>
       <c r="H35" s="27">
         <v>1</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2662,7 +2749,7 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="23">
         <v>1</v>
       </c>
       <c r="F36">
@@ -2682,7 +2769,7 @@
       <c r="D37">
         <v>1</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="23">
         <v>1</v>
       </c>
       <c r="F37">
@@ -2702,7 +2789,7 @@
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="23">
         <v>2</v>
       </c>
       <c r="F38">
@@ -2722,16 +2809,16 @@
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="E39" s="25">
-        <v>2</v>
-      </c>
-      <c r="F39" s="27">
-        <v>1</v>
-      </c>
-      <c r="G39" s="27">
-        <v>1</v>
-      </c>
-      <c r="H39" s="27">
+      <c r="E39" s="23">
+        <v>2</v>
+      </c>
+      <c r="F39" s="25">
+        <v>1</v>
+      </c>
+      <c r="G39" s="25">
+        <v>1</v>
+      </c>
+      <c r="H39" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2742,16 +2829,16 @@
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="23">
         <v>3</v>
       </c>
-      <c r="F40" s="27">
-        <v>2</v>
-      </c>
-      <c r="G40" s="27">
-        <v>2</v>
-      </c>
-      <c r="H40" s="27">
+      <c r="F40" s="25">
+        <v>2</v>
+      </c>
+      <c r="G40" s="25">
+        <v>2</v>
+      </c>
+      <c r="H40" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2762,16 +2849,16 @@
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="23">
         <v>3</v>
       </c>
-      <c r="F41" s="27">
-        <v>1</v>
-      </c>
-      <c r="G41" s="27">
-        <v>1</v>
-      </c>
-      <c r="H41" s="27">
+      <c r="F41" s="25">
+        <v>1</v>
+      </c>
+      <c r="G41" s="25">
+        <v>1</v>
+      </c>
+      <c r="H41" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2782,16 +2869,16 @@
       <c r="D42">
         <v>0</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="23">
         <v>4</v>
       </c>
-      <c r="F42" s="27">
-        <v>2</v>
-      </c>
-      <c r="G42" s="27">
-        <v>2</v>
-      </c>
-      <c r="H42" s="27">
+      <c r="F42" s="25">
+        <v>2</v>
+      </c>
+      <c r="G42" s="25">
+        <v>2</v>
+      </c>
+      <c r="H42" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2802,16 +2889,16 @@
       <c r="D43">
         <v>1</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="23">
         <v>4</v>
       </c>
-      <c r="F43" s="27">
-        <v>1</v>
-      </c>
-      <c r="G43" s="27">
-        <v>1</v>
-      </c>
-      <c r="H43" s="27">
+      <c r="F43" s="25">
+        <v>1</v>
+      </c>
+      <c r="G43" s="25">
+        <v>1</v>
+      </c>
+      <c r="H43" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2822,16 +2909,16 @@
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="23">
         <v>5</v>
       </c>
-      <c r="F44" s="27">
-        <v>2</v>
-      </c>
-      <c r="G44" s="27">
-        <v>2</v>
-      </c>
-      <c r="H44" s="27">
+      <c r="F44" s="25">
+        <v>2</v>
+      </c>
+      <c r="G44" s="25">
+        <v>2</v>
+      </c>
+      <c r="H44" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2842,16 +2929,16 @@
       <c r="D45">
         <v>1</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="23">
         <v>5</v>
       </c>
-      <c r="F45" s="27">
-        <v>1</v>
-      </c>
-      <c r="G45" s="27">
-        <v>1</v>
-      </c>
-      <c r="H45" s="27">
+      <c r="F45" s="25">
+        <v>1</v>
+      </c>
+      <c r="G45" s="25">
+        <v>1</v>
+      </c>
+      <c r="H45" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2862,16 +2949,16 @@
       <c r="D46">
         <v>0</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="23">
         <v>6</v>
       </c>
-      <c r="F46" s="27">
-        <v>2</v>
-      </c>
-      <c r="G46" s="27">
-        <v>2</v>
-      </c>
-      <c r="H46" s="27">
+      <c r="F46" s="25">
+        <v>2</v>
+      </c>
+      <c r="G46" s="25">
+        <v>2</v>
+      </c>
+      <c r="H46" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2882,16 +2969,16 @@
       <c r="D47">
         <v>1</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="23">
         <v>6</v>
       </c>
-      <c r="F47" s="27">
-        <v>1</v>
-      </c>
-      <c r="G47" s="27">
-        <v>1</v>
-      </c>
-      <c r="H47" s="27">
+      <c r="F47" s="25">
+        <v>1</v>
+      </c>
+      <c r="G47" s="25">
+        <v>1</v>
+      </c>
+      <c r="H47" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2902,16 +2989,16 @@
       <c r="D48">
         <v>0</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="23">
         <v>7</v>
       </c>
-      <c r="F48" s="27">
-        <v>2</v>
-      </c>
-      <c r="G48" s="27">
-        <v>2</v>
-      </c>
-      <c r="H48" s="27">
+      <c r="F48" s="25">
+        <v>2</v>
+      </c>
+      <c r="G48" s="25">
+        <v>2</v>
+      </c>
+      <c r="H48" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2922,16 +3009,16 @@
       <c r="D49">
         <v>1</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="23">
         <v>7</v>
       </c>
-      <c r="F49" s="27">
-        <v>1</v>
-      </c>
-      <c r="G49" s="27">
-        <v>1</v>
-      </c>
-      <c r="H49" s="27">
+      <c r="F49" s="25">
+        <v>1</v>
+      </c>
+      <c r="G49" s="25">
+        <v>1</v>
+      </c>
+      <c r="H49" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2942,16 +3029,16 @@
       <c r="D50">
         <v>0</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="23">
         <v>8</v>
       </c>
-      <c r="F50" s="27">
-        <v>2</v>
-      </c>
-      <c r="G50" s="27">
-        <v>2</v>
-      </c>
-      <c r="H50" s="27">
+      <c r="F50" s="25">
+        <v>2</v>
+      </c>
+      <c r="G50" s="25">
+        <v>2</v>
+      </c>
+      <c r="H50" s="25">
         <v>2</v>
       </c>
     </row>
@@ -2962,16 +3049,16 @@
       <c r="D51">
         <v>1</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="23">
         <v>8</v>
       </c>
-      <c r="F51" s="27">
-        <v>1</v>
-      </c>
-      <c r="G51" s="27">
-        <v>1</v>
-      </c>
-      <c r="H51" s="27">
+      <c r="F51" s="25">
+        <v>1</v>
+      </c>
+      <c r="G51" s="25">
+        <v>1</v>
+      </c>
+      <c r="H51" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2982,16 +3069,16 @@
       <c r="D52">
         <v>0</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="23">
         <v>9</v>
       </c>
-      <c r="F52" s="27">
-        <v>2</v>
-      </c>
-      <c r="G52" s="27">
-        <v>2</v>
-      </c>
-      <c r="H52" s="27">
+      <c r="F52" s="25">
+        <v>2</v>
+      </c>
+      <c r="G52" s="25">
+        <v>2</v>
+      </c>
+      <c r="H52" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3002,74 +3089,74 @@
       <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="23">
         <v>9</v>
       </c>
-      <c r="F53" s="27">
-        <v>1</v>
-      </c>
-      <c r="G53" s="27">
-        <v>1</v>
-      </c>
-      <c r="H53" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="29" customFormat="1">
-      <c r="A54" s="29">
+      <c r="F53" s="25">
+        <v>1</v>
+      </c>
+      <c r="G53" s="25">
+        <v>1</v>
+      </c>
+      <c r="H53" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="27" customFormat="1">
+      <c r="A54" s="27">
         <v>27</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="29">
-        <v>0</v>
-      </c>
-      <c r="E54" s="37">
+      <c r="D54" s="27">
+        <v>0</v>
+      </c>
+      <c r="E54" s="35">
         <v>10</v>
       </c>
-      <c r="F54" s="29">
-        <v>2</v>
-      </c>
-      <c r="G54" s="29">
-        <v>2</v>
-      </c>
-      <c r="H54" s="29">
-        <v>2</v>
-      </c>
-      <c r="I54" s="29" t="s">
+      <c r="F54" s="27">
+        <v>2</v>
+      </c>
+      <c r="G54" s="27">
+        <v>2</v>
+      </c>
+      <c r="H54" s="27">
+        <v>2</v>
+      </c>
+      <c r="I54" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="30" customFormat="1">
-      <c r="A55" s="30">
+    <row r="55" spans="1:9" s="28" customFormat="1">
+      <c r="A55" s="28">
         <v>27</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="30">
-        <v>1</v>
-      </c>
-      <c r="E55" s="35">
+      <c r="D55" s="28">
+        <v>1</v>
+      </c>
+      <c r="E55" s="33">
         <v>10</v>
       </c>
-      <c r="F55" s="30">
-        <v>1</v>
-      </c>
-      <c r="G55" s="30">
-        <v>1</v>
-      </c>
-      <c r="H55" s="30">
-        <v>1</v>
-      </c>
-      <c r="I55" s="30" t="s">
+      <c r="F55" s="28">
+        <v>1</v>
+      </c>
+      <c r="G55" s="28">
+        <v>1</v>
+      </c>
+      <c r="H55" s="28">
+        <v>1</v>
+      </c>
+      <c r="I55" s="28" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3080,16 +3167,16 @@
       <c r="D56">
         <v>0</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="23">
         <v>11</v>
       </c>
-      <c r="F56" s="27">
-        <v>2</v>
-      </c>
-      <c r="G56" s="27">
-        <v>2</v>
-      </c>
-      <c r="H56" s="27">
+      <c r="F56" s="25">
+        <v>2</v>
+      </c>
+      <c r="G56" s="25">
+        <v>2</v>
+      </c>
+      <c r="H56" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3100,16 +3187,16 @@
       <c r="D57">
         <v>1</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="23">
         <v>11</v>
       </c>
-      <c r="F57" s="27">
-        <v>1</v>
-      </c>
-      <c r="G57" s="27">
-        <v>1</v>
-      </c>
-      <c r="H57" s="27">
+      <c r="F57" s="25">
+        <v>1</v>
+      </c>
+      <c r="G57" s="25">
+        <v>1</v>
+      </c>
+      <c r="H57" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3120,16 +3207,16 @@
       <c r="D58">
         <v>0</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="23">
         <v>12</v>
       </c>
-      <c r="F58" s="27">
-        <v>2</v>
-      </c>
-      <c r="G58" s="27">
-        <v>2</v>
-      </c>
-      <c r="H58" s="27">
+      <c r="F58" s="25">
+        <v>2</v>
+      </c>
+      <c r="G58" s="25">
+        <v>2</v>
+      </c>
+      <c r="H58" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3140,16 +3227,16 @@
       <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="23">
         <v>12</v>
       </c>
-      <c r="F59" s="27">
-        <v>1</v>
-      </c>
-      <c r="G59" s="27">
-        <v>1</v>
-      </c>
-      <c r="H59" s="27">
+      <c r="F59" s="25">
+        <v>1</v>
+      </c>
+      <c r="G59" s="25">
+        <v>1</v>
+      </c>
+      <c r="H59" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3160,16 +3247,16 @@
       <c r="D60">
         <v>0</v>
       </c>
-      <c r="E60" s="25">
+      <c r="E60" s="23">
         <v>13</v>
       </c>
-      <c r="F60" s="27">
-        <v>2</v>
-      </c>
-      <c r="G60" s="27">
-        <v>2</v>
-      </c>
-      <c r="H60" s="27">
+      <c r="F60" s="25">
+        <v>2</v>
+      </c>
+      <c r="G60" s="25">
+        <v>2</v>
+      </c>
+      <c r="H60" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3180,16 +3267,16 @@
       <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="23">
         <v>13</v>
       </c>
-      <c r="F61" s="27">
-        <v>1</v>
-      </c>
-      <c r="G61" s="27">
-        <v>1</v>
-      </c>
-      <c r="H61" s="27">
+      <c r="F61" s="25">
+        <v>1</v>
+      </c>
+      <c r="G61" s="25">
+        <v>1</v>
+      </c>
+      <c r="H61" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3200,16 +3287,16 @@
       <c r="D62">
         <v>0</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="23">
         <v>14</v>
       </c>
-      <c r="F62" s="27">
-        <v>2</v>
-      </c>
-      <c r="G62" s="27">
-        <v>2</v>
-      </c>
-      <c r="H62" s="27">
+      <c r="F62" s="25">
+        <v>2</v>
+      </c>
+      <c r="G62" s="25">
+        <v>2</v>
+      </c>
+      <c r="H62" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3220,16 +3307,16 @@
       <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="23">
         <v>14</v>
       </c>
-      <c r="F63" s="27">
-        <v>1</v>
-      </c>
-      <c r="G63" s="27">
-        <v>1</v>
-      </c>
-      <c r="H63" s="27">
+      <c r="F63" s="25">
+        <v>1</v>
+      </c>
+      <c r="G63" s="25">
+        <v>1</v>
+      </c>
+      <c r="H63" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3240,16 +3327,16 @@
       <c r="D64">
         <v>0</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="23">
         <v>15</v>
       </c>
-      <c r="F64" s="27">
-        <v>2</v>
-      </c>
-      <c r="G64" s="27">
-        <v>2</v>
-      </c>
-      <c r="H64" s="27">
+      <c r="F64" s="25">
+        <v>2</v>
+      </c>
+      <c r="G64" s="25">
+        <v>2</v>
+      </c>
+      <c r="H64" s="25">
         <v>2</v>
       </c>
     </row>
@@ -3260,28 +3347,28 @@
       <c r="D65">
         <v>1</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="23">
         <v>15</v>
       </c>
-      <c r="F65" s="27">
-        <v>1</v>
-      </c>
-      <c r="G65" s="27">
-        <v>1</v>
-      </c>
-      <c r="H65" s="27">
+      <c r="F65" s="25">
+        <v>1</v>
+      </c>
+      <c r="G65" s="25">
+        <v>1</v>
+      </c>
+      <c r="H65" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="25"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="25"/>
+      <c r="H67" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes on the experiment arrangement
</commit_message>
<xml_diff>
--- a/Experiment Arrangements.xlsx
+++ b/Experiment Arrangements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ruoyu\MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF783348-7867-4508-B77B-26938C3046C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496FD545-0235-4A24-971C-3A520B38F4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latin Squares" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
   <si>
     <t>Col1</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t>12.Mar 15:00</t>
-  </si>
-  <si>
-    <t>19.Mar 13:00</t>
   </si>
   <si>
     <t>yasmeen.e.mahmoud@gmail.com</t>
@@ -264,6 +261,21 @@
   </si>
   <si>
     <t>12.Jun 17:00</t>
+  </si>
+  <si>
+    <t>Swaroopa Ganti</t>
+  </si>
+  <si>
+    <t>23.Jun 9:00</t>
+  </si>
+  <si>
+    <t>25.Jun 12:00</t>
+  </si>
+  <si>
+    <t>Bernhard Glas</t>
+  </si>
+  <si>
+    <t>23.Jun 11:00</t>
   </si>
 </sst>
 </file>
@@ -932,13 +944,13 @@
         <v>3</v>
       </c>
       <c r="N1" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1533,7 +1545,7 @@
         <v>8</v>
       </c>
       <c r="O17" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P17" s="40"/>
       <c r="Q17" s="40"/>
@@ -1765,8 +1777,8 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1932,6 +1944,12 @@
       <c r="A6">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
       <c r="D6">
         <v>1</v>
       </c>
@@ -1952,6 +1970,12 @@
       <c r="A7">
         <v>3</v>
       </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -2005,7 +2029,7 @@
         <v>57</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="24">
         <v>0</v>
@@ -2321,10 +2345,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="D20" s="24">
         <v>1</v>
@@ -2350,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -2374,10 +2398,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>65</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>66</v>
       </c>
       <c r="D22" s="28">
         <v>1</v>
@@ -2403,7 +2427,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2426,10 +2450,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="28">
         <v>1</v>
@@ -2455,7 +2479,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2510,7 +2534,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="24">
         <v>0</v>
@@ -2535,6 +2559,12 @@
       <c r="A28">
         <v>14</v>
       </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
       <c r="D28">
         <v>1</v>
       </c>
@@ -2555,6 +2585,9 @@
       <c r="A29">
         <v>14</v>
       </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
       <c r="D29">
         <v>0</v>
       </c>
@@ -2576,7 +2609,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>59</v>
@@ -2605,10 +2638,7 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2631,10 +2661,10 @@
         <v>16</v>
       </c>
       <c r="B32" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="D32" s="28">
         <v>1</v>
@@ -2660,10 +2690,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="24">
         <v>0</v>
@@ -2689,10 +2719,10 @@
         <v>17</v>
       </c>
       <c r="B34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>63</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>64</v>
       </c>
       <c r="D34" s="29">
         <v>0</v>
@@ -2718,10 +2748,10 @@
         <v>17</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35" s="24">
         <v>1</v>

</xml_diff>

<commit_message>
More experiments and more arrangements
</commit_message>
<xml_diff>
--- a/Experiment Arrangements.xlsx
+++ b/Experiment Arrangements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ruoyu\MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5A8BF7-B226-4F14-B418-202EBAC9B15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52607E0D-51F7-43D2-9158-A17B8E0269B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latin Squares" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="88">
   <si>
     <t>Col1</t>
   </si>
@@ -290,7 +290,13 @@
     <t>Ahmed Shams</t>
   </si>
   <si>
-    <t>23.Jun 12:00</t>
+    <t>25.Jun 9:00</t>
+  </si>
+  <si>
+    <t>25.Jun 10:00</t>
+  </si>
+  <si>
+    <t>30.Jun 12:00</t>
   </si>
 </sst>
 </file>
@@ -638,11 +644,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -927,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1561,11 +1567,11 @@
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="O17" s="40" t="s">
+      <c r="O17" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="21">
@@ -1606,9 +1612,9 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="21">
@@ -1649,9 +1655,9 @@
         <f>H11</f>
         <v>0</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="21">
@@ -1692,9 +1698,9 @@
         <f t="shared" ref="K20:K22" si="15">H12</f>
         <v>1</v>
       </c>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="21">
@@ -1735,9 +1741,9 @@
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="22">
@@ -1793,9 +1799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F24D3-6BE6-4CB6-9FA7-79DC1B6507FC}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1957,30 +1963,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    <row r="6" spans="1:10" s="24" customFormat="1">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="23">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
+      <c r="D6" s="24">
+        <v>1</v>
+      </c>
+      <c r="E6" s="24">
+        <v>2</v>
+      </c>
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24">
+        <v>1</v>
+      </c>
+      <c r="H6" s="24">
+        <v>1</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2580,7 +2589,7 @@
         <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3390,59 +3399,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="3" customFormat="1">
+    <row r="65" spans="1:9" s="3" customFormat="1">
       <c r="A65" s="3">
         <v>32</v>
       </c>
       <c r="D65" s="3">
         <v>1</v>
       </c>
-      <c r="E65" s="41">
+      <c r="E65" s="40">
         <v>15</v>
       </c>
-      <c r="F65" s="42">
-        <v>1</v>
-      </c>
-      <c r="G65" s="42">
-        <v>1</v>
-      </c>
-      <c r="H65" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66">
+      <c r="F65" s="41">
+        <v>1</v>
+      </c>
+      <c r="G65" s="41">
+        <v>1</v>
+      </c>
+      <c r="H65" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="24" customFormat="1">
+      <c r="A66" s="24">
         <v>33</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66" s="23">
-        <v>0</v>
-      </c>
-      <c r="F66" s="25">
-        <v>2</v>
-      </c>
-      <c r="G66" s="25">
-        <v>2</v>
-      </c>
-      <c r="H66" s="25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="D66" s="24">
+        <v>1</v>
+      </c>
+      <c r="E66" s="24">
+        <v>0</v>
+      </c>
+      <c r="F66" s="27">
+        <v>2</v>
+      </c>
+      <c r="G66" s="27">
+        <v>2</v>
+      </c>
+      <c r="H66" s="27">
+        <v>2</v>
+      </c>
+      <c r="I66" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>33</v>
       </c>
       <c r="B67" t="s">
         <v>82</v>
       </c>
+      <c r="C67" t="s">
+        <v>85</v>
+      </c>
       <c r="D67">
         <v>0</v>
       </c>
@@ -3459,39 +3474,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68">
+    <row r="68" spans="1:9" s="24" customFormat="1">
+      <c r="A68" s="24">
         <v>34</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C68" t="s">
-        <v>85</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68" s="23">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <v>2</v>
-      </c>
-      <c r="G68">
-        <v>2</v>
-      </c>
-      <c r="H68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="C68" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="24">
+        <v>1</v>
+      </c>
+      <c r="E68" s="24">
+        <v>1</v>
+      </c>
+      <c r="F68" s="24">
+        <v>2</v>
+      </c>
+      <c r="G68" s="24">
+        <v>2</v>
+      </c>
+      <c r="H68" s="24">
+        <v>2</v>
+      </c>
+      <c r="I68" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>34</v>
       </c>
       <c r="B69" t="s">
         <v>84</v>
       </c>
+      <c r="C69" t="s">
+        <v>86</v>
+      </c>
       <c r="D69">
         <v>0</v>
       </c>
@@ -3508,7 +3529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>35</v>
       </c>
@@ -3528,7 +3549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>35</v>
       </c>
@@ -3548,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>36</v>
       </c>
@@ -3568,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>36</v>
       </c>
@@ -3588,7 +3609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>37</v>
       </c>
@@ -3608,7 +3629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>37</v>
       </c>
@@ -3628,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>38</v>
       </c>
@@ -3648,7 +3669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>38</v>
       </c>
@@ -3668,7 +3689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>39</v>
       </c>
@@ -3688,7 +3709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>39</v>
       </c>
@@ -3708,7 +3729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
A lot more experiments
</commit_message>
<xml_diff>
--- a/Experiment Arrangements.xlsx
+++ b/Experiment Arrangements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ruoyu\MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E04F50-0A98-4B59-B11E-2B56229BF53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BDF10A-226B-41A6-9800-4E2366FF4B6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Latin Squares" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="99">
   <si>
     <t>Col1</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Alaa Musleh</t>
   </si>
   <si>
-    <t>Syamala Kovvuri</t>
-  </si>
-  <si>
     <t>09.July 11:45</t>
   </si>
   <si>
@@ -312,6 +309,27 @@
   </si>
   <si>
     <t>14.July 16:00</t>
+  </si>
+  <si>
+    <t>Rahul Choubey</t>
+  </si>
+  <si>
+    <t>16.July 11:00</t>
+  </si>
+  <si>
+    <t>Sonia Gonzales</t>
+  </si>
+  <si>
+    <t>16.July 13:00</t>
+  </si>
+  <si>
+    <t>Moeen Khurram</t>
+  </si>
+  <si>
+    <t>16.July 15:00</t>
+  </si>
+  <si>
+    <t>16.July 12:20</t>
   </si>
 </sst>
 </file>
@@ -949,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17:Q21"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1815,9 +1833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7F24D3-6BE6-4CB6-9FA7-79DC1B6507FC}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2683,7 +2701,7 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2831,7 +2849,7 @@
         <v>87</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D36" s="24">
         <v>0</v>
@@ -2852,99 +2870,117 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37">
+    <row r="37" spans="1:10" s="24" customFormat="1">
+      <c r="A37" s="24">
         <v>18</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="23">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38">
+      <c r="C37" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="24">
+        <v>1</v>
+      </c>
+      <c r="E37" s="24">
+        <v>1</v>
+      </c>
+      <c r="F37" s="24">
+        <v>1</v>
+      </c>
+      <c r="G37" s="24">
+        <v>1</v>
+      </c>
+      <c r="H37" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="24" customFormat="1">
+      <c r="A38" s="24">
         <v>19</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38" s="23">
-        <v>2</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
-        <v>2</v>
-      </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39">
+      <c r="D38" s="24">
+        <v>0</v>
+      </c>
+      <c r="E38" s="24">
+        <v>2</v>
+      </c>
+      <c r="F38" s="24">
+        <v>2</v>
+      </c>
+      <c r="G38" s="24">
+        <v>2</v>
+      </c>
+      <c r="H38" s="24">
+        <v>2</v>
+      </c>
+      <c r="I38" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="24" customFormat="1">
+      <c r="A39" s="24">
         <v>19</v>
       </c>
-      <c r="B39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="23">
-        <v>2</v>
-      </c>
-      <c r="F39" s="25">
-        <v>1</v>
-      </c>
-      <c r="G39" s="25">
-        <v>1</v>
-      </c>
-      <c r="H39" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40">
+      <c r="B39" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="24">
+        <v>1</v>
+      </c>
+      <c r="E39" s="24">
+        <v>2</v>
+      </c>
+      <c r="F39" s="27">
+        <v>1</v>
+      </c>
+      <c r="G39" s="27">
+        <v>1</v>
+      </c>
+      <c r="H39" s="27">
+        <v>1</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="24" customFormat="1">
+      <c r="A40" s="24">
         <v>20</v>
       </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" s="23">
+      <c r="B40" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
+      <c r="E40" s="24">
         <v>3</v>
       </c>
-      <c r="F40" s="25">
-        <v>2</v>
-      </c>
-      <c r="G40" s="25">
-        <v>2</v>
-      </c>
-      <c r="H40" s="25">
-        <v>2</v>
+      <c r="F40" s="27">
+        <v>2</v>
+      </c>
+      <c r="G40" s="27">
+        <v>2</v>
+      </c>
+      <c r="H40" s="27">
+        <v>2</v>
+      </c>
+      <c r="I40" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2952,7 +2988,7 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2970,30 +3006,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42">
+    <row r="42" spans="1:10" s="24" customFormat="1">
+      <c r="A42" s="24">
         <v>21</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" s="23">
+      <c r="B42" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="24">
+        <v>0</v>
+      </c>
+      <c r="E42" s="24">
         <v>4</v>
       </c>
-      <c r="F42" s="25">
-        <v>2</v>
-      </c>
-      <c r="G42" s="25">
-        <v>2</v>
-      </c>
-      <c r="H42" s="25">
-        <v>2</v>
+      <c r="F42" s="27">
+        <v>2</v>
+      </c>
+      <c r="G42" s="27">
+        <v>2</v>
+      </c>
+      <c r="H42" s="27">
+        <v>2</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
         <v>21</v>
       </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
       <c r="D43">
         <v>1</v>
       </c>
@@ -3014,25 +3062,31 @@
       <c r="A44">
         <v>22</v>
       </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44" s="23">
+      <c r="E44">
         <v>5</v>
       </c>
-      <c r="F44" s="25">
-        <v>2</v>
-      </c>
-      <c r="G44" s="25">
-        <v>2</v>
-      </c>
-      <c r="H44" s="25">
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
         <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
       </c>
       <c r="D45">
         <v>1</v>

</xml_diff>

<commit_message>
More experiments and changes
</commit_message>
<xml_diff>
--- a/Experiment Arrangements.xlsx
+++ b/Experiment Arrangements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ruoyu\MasterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57E7FF5-769E-4AF7-9A5D-03F8E4FFD3AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF3FBFF-BB8B-48FE-BB15-CEDFA78883DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="137">
   <si>
     <t>Col1</t>
   </si>
@@ -227,9 +221,6 @@
   </si>
   <si>
     <t>Anqi Wang</t>
-  </si>
-  <si>
-    <t>15.Mar</t>
   </si>
   <si>
     <t>Zhihan Jiang</t>
@@ -392,9 +383,6 @@
     <t>04.Aug 15:00</t>
   </si>
   <si>
-    <t>Accidently set id to be 23 which has been done already on another person</t>
-  </si>
-  <si>
     <t>04.Aug 11:00</t>
   </si>
   <si>
@@ -402,13 +390,61 @@
   </si>
   <si>
     <t>04.Aug 12:00</t>
+  </si>
+  <si>
+    <t>06.Aug 10:00</t>
+  </si>
+  <si>
+    <t>Sinan Emre Güler</t>
+  </si>
+  <si>
+    <t>06.Aug 11:00</t>
+  </si>
+  <si>
+    <t>06.Aug 12:00</t>
+  </si>
+  <si>
+    <t>06.Aug 14:00</t>
+  </si>
+  <si>
+    <t>06.Aug 15:00</t>
+  </si>
+  <si>
+    <t>06.Aug 13:00</t>
+  </si>
+  <si>
+    <t>Marko Begic</t>
+  </si>
+  <si>
+    <t>11.Aug 9:00</t>
+  </si>
+  <si>
+    <t>11.Aug 11:00</t>
+  </si>
+  <si>
+    <t>Celia Borja Almarcha</t>
+  </si>
+  <si>
+    <t>11.Aug 17:00</t>
+  </si>
+  <si>
+    <t>Accidently set id to be 23 (should be 24) which belonged to another person</t>
+  </si>
+  <si>
+    <t>15.Mar 17:00</t>
+  </si>
+  <si>
+    <t>15.Mar 18:00</t>
+  </si>
+  <si>
+    <t>11.Aug 16:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,8 +512,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +541,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -712,13 +761,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -763,14 +813,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
@@ -1086,13 +1138,13 @@
         <v>3</v>
       </c>
       <c r="N1" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1686,11 +1738,11 @@
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="O17" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
+      <c r="O17" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="21">
@@ -1731,9 +1783,9 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="21">
@@ -1774,9 +1826,9 @@
         <f>H11</f>
         <v>0</v>
       </c>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="21">
@@ -1817,9 +1869,9 @@
         <f t="shared" ref="K20:K22" si="15">H12</f>
         <v>1</v>
       </c>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="21">
@@ -1860,9 +1912,9 @@
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="22">
@@ -1919,8 +1971,8 @@
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2090,10 +2142,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>76</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>77</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
@@ -2119,10 +2171,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="26">
         <v>0</v>
@@ -2180,7 +2232,7 @@
         <v>57</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="26">
         <v>0</v>
@@ -2552,7 +2604,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="D22" s="26">
         <v>1</v>
@@ -2573,78 +2625,81 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1">
-      <c r="A23" s="1">
+    <row r="23" spans="1:10" s="43" customFormat="1">
+      <c r="A23" s="43">
         <v>11</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="39">
+      <c r="C23" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0</v>
+      </c>
+      <c r="E23" s="43">
         <v>10</v>
       </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="26" customFormat="1">
-      <c r="A24" s="26">
+      <c r="F23" s="43">
+        <v>2</v>
+      </c>
+      <c r="G23" s="43">
+        <v>2</v>
+      </c>
+      <c r="H23" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="41" customFormat="1">
+      <c r="A24" s="41">
         <v>12</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="26">
-        <v>1</v>
-      </c>
-      <c r="E24" s="31">
+      <c r="C24" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="41">
+        <v>1</v>
+      </c>
+      <c r="E24" s="41">
         <v>11</v>
       </c>
-      <c r="F24" s="26">
-        <v>1</v>
-      </c>
-      <c r="G24" s="26">
-        <v>1</v>
-      </c>
-      <c r="H24" s="26">
-        <v>1</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="1" customFormat="1">
-      <c r="A25" s="1">
+      <c r="F24" s="41">
+        <v>1</v>
+      </c>
+      <c r="G24" s="41">
+        <v>1</v>
+      </c>
+      <c r="H24" s="41">
+        <v>1</v>
+      </c>
+      <c r="I24" s="41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="41" customFormat="1">
+      <c r="A25" s="41">
         <v>12</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="39">
+      <c r="B25" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="41">
+        <v>0</v>
+      </c>
+      <c r="E25" s="41">
         <v>11</v>
       </c>
-      <c r="F25" s="1">
-        <v>2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="41">
+        <v>2</v>
+      </c>
+      <c r="G25" s="41">
+        <v>2</v>
+      </c>
+      <c r="H25" s="41">
         <v>2</v>
       </c>
     </row>
@@ -2685,7 +2740,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="24">
         <v>0</v>
@@ -2711,10 +2766,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>102</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>103</v>
       </c>
       <c r="D28" s="24">
         <v>1</v>
@@ -2740,10 +2795,10 @@
         <v>14</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" s="24">
         <v>0</v>
@@ -2769,7 +2824,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>59</v>
@@ -2798,10 +2853,10 @@
         <v>15</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="24">
         <v>0</v>
@@ -2822,7 +2877,7 @@
         <v>54</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="26" customFormat="1">
@@ -2830,10 +2885,10 @@
         <v>16</v>
       </c>
       <c r="B32" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>68</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>69</v>
       </c>
       <c r="D32" s="26">
         <v>1</v>
@@ -2859,10 +2914,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D33" s="24">
         <v>0</v>
@@ -2920,7 +2975,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="24">
         <v>1</v>
@@ -2941,7 +2996,7 @@
         <v>54</v>
       </c>
       <c r="J35" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="24" customFormat="1">
@@ -2949,10 +3004,10 @@
         <v>18</v>
       </c>
       <c r="B36" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>87</v>
       </c>
       <c r="D36" s="24">
         <v>0</v>
@@ -2978,10 +3033,10 @@
         <v>18</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="24">
         <v>1</v>
@@ -3007,10 +3062,10 @@
         <v>19</v>
       </c>
       <c r="B38" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="24" t="s">
         <v>88</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>89</v>
       </c>
       <c r="D38" s="24">
         <v>0</v>
@@ -3036,10 +3091,10 @@
         <v>19</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="24">
         <v>1</v>
@@ -3065,10 +3120,10 @@
         <v>20</v>
       </c>
       <c r="B40" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>91</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>92</v>
       </c>
       <c r="D40" s="24">
         <v>0</v>
@@ -3094,10 +3149,10 @@
         <v>20</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="24">
         <v>1</v>
@@ -3123,10 +3178,10 @@
         <v>21</v>
       </c>
       <c r="B42" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>94</v>
       </c>
       <c r="D42" s="26">
         <v>0</v>
@@ -3152,10 +3207,10 @@
         <v>21</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D43" s="26">
         <v>1</v>
@@ -3181,10 +3236,10 @@
         <v>22</v>
       </c>
       <c r="B44" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="D44" s="26">
         <v>0</v>
@@ -3210,10 +3265,10 @@
         <v>22</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" s="26">
         <v>1</v>
@@ -3239,10 +3294,10 @@
         <v>23</v>
       </c>
       <c r="B46" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="26" t="s">
         <v>108</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>109</v>
       </c>
       <c r="D46" s="26">
         <v>0</v>
@@ -3263,27 +3318,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1">
-      <c r="A47" s="1">
+    <row r="47" spans="1:10" s="26" customFormat="1">
+      <c r="A47" s="26">
         <v>23</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="39">
+      <c r="B47" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="26">
+        <v>1</v>
+      </c>
+      <c r="E47" s="26">
         <v>6</v>
       </c>
-      <c r="F47" s="25">
-        <v>1</v>
-      </c>
-      <c r="G47" s="25">
-        <v>1</v>
-      </c>
-      <c r="H47" s="25">
-        <v>1</v>
+      <c r="F47" s="26">
+        <v>1</v>
+      </c>
+      <c r="G47" s="26">
+        <v>1</v>
+      </c>
+      <c r="H47" s="26">
+        <v>1</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="26" customFormat="1">
@@ -3291,10 +3352,10 @@
         <v>24</v>
       </c>
       <c r="B48" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="26" t="s">
         <v>97</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>98</v>
       </c>
       <c r="D48" s="26">
         <v>0</v>
@@ -3320,10 +3381,10 @@
         <v>24</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D49" s="26">
         <v>1</v>
@@ -3349,10 +3410,10 @@
         <v>25</v>
       </c>
       <c r="B50" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="26" t="s">
         <v>112</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>113</v>
       </c>
       <c r="D50" s="26">
         <v>0</v>
@@ -3373,27 +3434,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="1" customFormat="1">
-      <c r="A51" s="1">
+    <row r="51" spans="1:9" s="26" customFormat="1">
+      <c r="A51" s="26">
         <v>25</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="39">
+      <c r="B51" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="26">
+        <v>1</v>
+      </c>
+      <c r="E51" s="26">
         <v>8</v>
       </c>
-      <c r="F51" s="25">
-        <v>1</v>
-      </c>
-      <c r="G51" s="25">
-        <v>1</v>
-      </c>
-      <c r="H51" s="25">
-        <v>1</v>
+      <c r="F51" s="26">
+        <v>1</v>
+      </c>
+      <c r="G51" s="26">
+        <v>1</v>
+      </c>
+      <c r="H51" s="26">
+        <v>1</v>
+      </c>
+      <c r="I51" s="26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="26" customFormat="1">
@@ -3401,10 +3468,10 @@
         <v>26</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D52" s="26">
         <v>0</v>
@@ -3425,27 +3492,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1">
-      <c r="A53" s="1">
+    <row r="53" spans="1:9" s="26" customFormat="1">
+      <c r="A53" s="26">
         <v>26</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" s="39">
+      <c r="B53" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53" s="26">
+        <v>1</v>
+      </c>
+      <c r="E53" s="26">
         <v>9</v>
       </c>
-      <c r="F53" s="25">
-        <v>1</v>
-      </c>
-      <c r="G53" s="25">
-        <v>1</v>
-      </c>
-      <c r="H53" s="25">
-        <v>1</v>
+      <c r="F53" s="26">
+        <v>1</v>
+      </c>
+      <c r="G53" s="26">
+        <v>1</v>
+      </c>
+      <c r="H53" s="26">
+        <v>1</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="26" customFormat="1">
@@ -3511,10 +3584,10 @@
         <v>28</v>
       </c>
       <c r="B56" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>116</v>
       </c>
       <c r="D56" s="26">
         <v>0</v>
@@ -3540,7 +3613,7 @@
         <v>28</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
@@ -3563,10 +3636,10 @@
         <v>29</v>
       </c>
       <c r="B58" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="26" t="s">
         <v>117</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="D58" s="26">
         <v>0</v>
@@ -3587,27 +3660,33 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="1" customFormat="1">
-      <c r="A59" s="1">
+    <row r="59" spans="1:9" s="26" customFormat="1">
+      <c r="A59" s="26">
         <v>29</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1</v>
-      </c>
-      <c r="E59" s="39">
+      <c r="B59" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="26">
+        <v>1</v>
+      </c>
+      <c r="E59" s="26">
         <v>12</v>
       </c>
-      <c r="F59" s="25">
-        <v>1</v>
-      </c>
-      <c r="G59" s="25">
-        <v>1</v>
-      </c>
-      <c r="H59" s="25">
-        <v>1</v>
+      <c r="F59" s="26">
+        <v>1</v>
+      </c>
+      <c r="G59" s="26">
+        <v>1</v>
+      </c>
+      <c r="H59" s="26">
+        <v>1</v>
+      </c>
+      <c r="I59" s="26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="26" customFormat="1">
@@ -3615,10 +3694,10 @@
         <v>30</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D60" s="26">
         <v>0</v>
@@ -3639,106 +3718,136 @@
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61">
+    <row r="61" spans="1:9" s="24" customFormat="1">
+      <c r="A61" s="24">
         <v>30</v>
       </c>
-      <c r="B61" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
+      <c r="B61" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D61" s="24">
+        <v>1</v>
+      </c>
+      <c r="E61" s="24">
         <v>13</v>
       </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="41" customFormat="1">
-      <c r="A62" s="41">
+      <c r="F61" s="24">
+        <v>1</v>
+      </c>
+      <c r="G61" s="24">
+        <v>1</v>
+      </c>
+      <c r="H61" s="24">
+        <v>1</v>
+      </c>
+      <c r="I61" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="24" customFormat="1">
+      <c r="A62" s="24">
         <v>31</v>
       </c>
-      <c r="D62" s="41">
-        <v>0</v>
-      </c>
-      <c r="E62" s="41">
+      <c r="B62" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="24">
+        <v>0</v>
+      </c>
+      <c r="E62" s="24">
         <v>14</v>
       </c>
-      <c r="F62" s="41">
-        <v>2</v>
-      </c>
-      <c r="G62" s="41">
-        <v>2</v>
-      </c>
-      <c r="H62" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="41" customFormat="1">
-      <c r="A63" s="41">
+      <c r="F62" s="24">
+        <v>2</v>
+      </c>
+      <c r="G62" s="24">
+        <v>2</v>
+      </c>
+      <c r="H62" s="24">
+        <v>2</v>
+      </c>
+      <c r="I62" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63">
         <v>31</v>
       </c>
-      <c r="D63" s="41">
-        <v>1</v>
-      </c>
-      <c r="E63" s="41">
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
         <v>14</v>
       </c>
-      <c r="F63" s="41">
-        <v>1</v>
-      </c>
-      <c r="G63" s="41">
-        <v>1</v>
-      </c>
-      <c r="H63" s="41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="41" customFormat="1">
-      <c r="A64" s="41">
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="24" customFormat="1">
+      <c r="A64" s="24">
         <v>32</v>
       </c>
-      <c r="D64" s="41">
-        <v>0</v>
-      </c>
-      <c r="E64" s="41">
+      <c r="B64" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="24">
+        <v>0</v>
+      </c>
+      <c r="E64" s="24">
         <v>15</v>
       </c>
-      <c r="F64" s="41">
-        <v>2</v>
-      </c>
-      <c r="G64" s="41">
-        <v>2</v>
-      </c>
-      <c r="H64" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="42" customFormat="1">
-      <c r="A65" s="42">
+      <c r="F64" s="24">
+        <v>2</v>
+      </c>
+      <c r="G64" s="24">
+        <v>2</v>
+      </c>
+      <c r="H64" s="24">
+        <v>2</v>
+      </c>
+      <c r="I64" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
         <v>32</v>
       </c>
-      <c r="D65" s="42">
-        <v>1</v>
-      </c>
-      <c r="E65" s="42">
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
         <v>15</v>
       </c>
-      <c r="F65" s="42">
-        <v>1</v>
-      </c>
-      <c r="G65" s="42">
-        <v>1</v>
-      </c>
-      <c r="H65" s="42">
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
         <v>1</v>
       </c>
     </row>
@@ -3747,10 +3856,10 @@
         <v>33</v>
       </c>
       <c r="B66" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="24" t="s">
         <v>81</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="D66" s="24">
         <v>1</v>
@@ -3776,10 +3885,10 @@
         <v>33</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -3805,10 +3914,10 @@
         <v>34</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D68" s="24">
         <v>1</v>
@@ -3834,10 +3943,10 @@
         <v>34</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D69" s="24">
         <v>0</v>
@@ -4418,43 +4527,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="40" customFormat="1">
-      <c r="A98" s="41">
+    <row r="98" spans="1:10" s="42" customFormat="1">
+      <c r="A98" s="42">
         <v>49</v>
       </c>
-      <c r="D98" s="40">
-        <v>0</v>
-      </c>
-      <c r="E98" s="40">
-        <v>0</v>
-      </c>
-      <c r="F98" s="40">
-        <v>1</v>
-      </c>
-      <c r="G98" s="40">
-        <v>1</v>
-      </c>
-      <c r="H98" s="40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" s="40" customFormat="1">
-      <c r="A99" s="41">
+      <c r="B98" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C98" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D98" s="42">
+        <v>0</v>
+      </c>
+      <c r="E98" s="42">
+        <v>0</v>
+      </c>
+      <c r="F98" s="42">
+        <v>1</v>
+      </c>
+      <c r="G98" s="42">
+        <v>1</v>
+      </c>
+      <c r="H98" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
         <v>49</v>
       </c>
-      <c r="D99" s="40">
-        <v>1</v>
-      </c>
-      <c r="E99" s="40">
-        <v>0</v>
-      </c>
-      <c r="F99" s="40">
-        <v>2</v>
-      </c>
-      <c r="G99" s="40">
-        <v>2</v>
-      </c>
-      <c r="H99" s="40">
+      <c r="B99" t="s">
+        <v>131</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99">
         <v>2</v>
       </c>
     </row>
@@ -4498,59 +4616,105 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="40" customFormat="1">
-      <c r="A108" s="40">
-        <v>55</v>
-      </c>
-      <c r="B108" s="40" t="s">
+    <row r="105" spans="1:10" s="40" customFormat="1">
+      <c r="A105" s="40">
+        <v>71</v>
+      </c>
+      <c r="D105" s="41">
+        <v>1</v>
+      </c>
+      <c r="E105" s="41">
+        <v>6</v>
+      </c>
+      <c r="F105" s="41">
+        <v>1</v>
+      </c>
+      <c r="G105" s="41">
+        <v>1</v>
+      </c>
+      <c r="H105" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="40" customFormat="1">
+      <c r="A106" s="40">
+        <v>71</v>
+      </c>
+      <c r="D106" s="41">
+        <v>0</v>
+      </c>
+      <c r="E106" s="41">
+        <v>6</v>
+      </c>
+      <c r="F106" s="41">
+        <v>2</v>
+      </c>
+      <c r="G106" s="41">
+        <v>2</v>
+      </c>
+      <c r="H106" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="24" customFormat="1">
+      <c r="A108" s="24">
+        <v>87</v>
+      </c>
+      <c r="B108" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C108" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D108" s="40">
-        <v>0</v>
-      </c>
-      <c r="E108" s="40">
+      <c r="D108" s="24">
+        <v>0</v>
+      </c>
+      <c r="E108" s="24">
         <v>6</v>
       </c>
-      <c r="F108" s="40">
-        <v>2</v>
-      </c>
-      <c r="G108" s="40">
-        <v>2</v>
-      </c>
-      <c r="H108" s="40">
-        <v>2</v>
-      </c>
-      <c r="I108" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="J108" s="40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" s="40" customFormat="1">
-      <c r="A109" s="40">
-        <v>55</v>
-      </c>
-      <c r="B109" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="D109" s="40">
-        <v>1</v>
-      </c>
-      <c r="E109" s="40">
+      <c r="F108" s="24">
+        <v>2</v>
+      </c>
+      <c r="G108" s="24">
+        <v>2</v>
+      </c>
+      <c r="H108" s="24">
+        <v>2</v>
+      </c>
+      <c r="I108" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="J108" s="24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="24" customFormat="1">
+      <c r="A109" s="24">
+        <v>87</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D109" s="24">
+        <v>1</v>
+      </c>
+      <c r="E109" s="24">
         <v>6</v>
       </c>
-      <c r="F109" s="41">
-        <v>1</v>
-      </c>
-      <c r="G109" s="41">
-        <v>1</v>
-      </c>
-      <c r="H109" s="41">
-        <v>1</v>
+      <c r="F109" s="26">
+        <v>1</v>
+      </c>
+      <c r="G109" s="26">
+        <v>1</v>
+      </c>
+      <c r="H109" s="26">
+        <v>1</v>
+      </c>
+      <c r="I109" s="24" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>